<commit_message>
DEV-22 remove redundant comments
</commit_message>
<xml_diff>
--- a/src/Shared/excel_retriever/infra/excelDownloaded.xlsx
+++ b/src/Shared/excel_retriever/infra/excelDownloaded.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="BOARD Hoja 1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="BOARD Hoja 2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="BOARD Hoja 3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Copia de BOARD Hoja 3 2" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Copia de BOARD Hoja 3" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="8">
   <si>
     <t>Tue Oct 18 17:38:42 2022</t>
   </si>
@@ -26,6 +26,18 @@
   </si>
   <si>
     <t>[TABLE] NOMBRE2</t>
+  </si>
+  <si>
+    <t>bruh</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -737,7 +749,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -819,7 +833,9 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3">
+        <v>1.0</v>
+      </c>
       <c r="B10" s="1">
         <v>1.0</v>
       </c>
@@ -861,9 +877,6 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
@@ -872,18 +885,6 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="2"/>
@@ -892,44 +893,68 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="1">
+    </row>
+    <row r="18">
+      <c r="G18" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="1">
         <v>4.0</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H20" s="1">
         <v>4.0</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I20" s="1">
         <v>4.0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="G15" s="1">
+    <row r="21">
+      <c r="G21" s="1">
         <v>5.0</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H21" s="1">
         <v>5.0</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I21" s="1">
         <v>5.0</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J21" s="5">
         <v>5.0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="G16" s="1">
+    <row r="22">
+      <c r="G22" s="1">
         <v>6.0</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H22" s="1">
         <v>6.0</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I22" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="J22" s="5">
         <v>6.0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G18:J18"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>